<commit_message>
created a way to compare bilevel and iterative
</commit_message>
<xml_diff>
--- a/timing of model improvements.xlsx
+++ b/timing of model improvements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frede\Documents\DTU\2024\MSc 3. semester\Optimization in Modern Power Systems\optimization_46750\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045AD41F-30F5-40C2-B9E7-269D7E9E31FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96427CFD-6D09-4620-BEAD-A54662C6C667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CA1CAD92-8D7E-4566-88E5-5892C930C84C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Bilevel speed up measures</t>
   </si>
@@ -48,18 +48,6 @@
   </si>
   <si>
     <t>Hours run</t>
-  </si>
-  <si>
-    <t>2 hours</t>
-  </si>
-  <si>
-    <t>base model</t>
-  </si>
-  <si>
-    <t>2 hours - improved bounds</t>
-  </si>
-  <si>
-    <t>2 hours - lambda bounds</t>
   </si>
   <si>
     <t>Objective value [M€]</t>
@@ -310,143 +298,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>542115</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>86247</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{827B849F-01FF-DB9E-DE2B-1D4B812EF2F6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7498080" y="1280160"/>
-          <a:ext cx="7849695" cy="3743847"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>142010</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>105194</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57644C62-1EC1-7BED-4BE1-CCDADA7FE496}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7498080" y="5334000"/>
-          <a:ext cx="7449590" cy="3000794"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>572516</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E9AB294-42C8-0506-6636-95C7849E6CA1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7490460" y="8595360"/>
-          <a:ext cx="7278116" cy="3010320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9CC6BA-B728-4C66-9042-34AB7ADD0A81}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,22 +634,22 @@
     <col min="7" max="7" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
@@ -809,21 +660,21 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -831,14 +682,8 @@
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
       <c r="H5" s="3"/>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="11">
         <v>1</v>
       </c>
@@ -861,7 +706,7 @@
         <v>232.9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="11">
         <v>2</v>
       </c>
@@ -884,7 +729,7 @@
         <v>216.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>5</v>
       </c>
@@ -894,18 +739,20 @@
       <c r="G8" s="5">
         <v>118.26</v>
       </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H8" s="5">
+        <v>133.30000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="11">
         <v>24</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -914,7 +761,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="11">
         <v>1</v>
       </c>
@@ -934,7 +781,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>2</v>
       </c>
@@ -954,7 +801,7 @@
         <v>6.36</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>5</v>
       </c>
@@ -965,15 +812,15 @@
         <v>117.68</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>24</v>
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -981,7 +828,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
         <v>1</v>
       </c>
@@ -1006,7 +853,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <v>2</v>
       </c>
@@ -1031,7 +878,7 @@
         <v>0.37000000000000011</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
         <v>5</v>
       </c>
@@ -1056,7 +903,7 @@
         <v>0.57999999999999829</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="11">
         <v>24</v>
       </c>
@@ -1081,9 +928,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -1091,7 +938,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>1</v>
       </c>
@@ -1111,7 +958,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
         <v>2</v>
       </c>
@@ -1131,7 +978,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
         <v>5</v>
       </c>
@@ -1141,19 +988,16 @@
       <c r="G23" s="5">
         <v>39.93</v>
       </c>
-      <c r="J23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <v>24</v>
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -1161,7 +1005,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
         <v>1</v>
       </c>
@@ -1186,7 +1030,7 @@
         <v>6.0526315789473681</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="11">
         <v>2</v>
       </c>
@@ -1211,7 +1055,7 @@
         <v>4.8549618320610683</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
         <v>5</v>
       </c>
@@ -1236,7 +1080,7 @@
         <v>2.9471575256699225</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="18">
         <v>24</v>
       </c>
@@ -1261,38 +1105,32 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J41" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>